<commit_message>
facing token added for new tokens
</commit_message>
<xml_diff>
--- a/Skillsets.xlsx
+++ b/Skillsets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D031A7-6C89-41E9-BCF0-C803FB0A6CBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8271369-13C2-43F0-BD8E-4FDD20F8DE53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{94108416-7DA5-4E31-B1F3-D159934FD6B5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="182">
   <si>
     <t>Hand Seal</t>
   </si>
@@ -388,9 +388,6 @@
     <t>When two hands are free, gain +2 hand seals per turn.</t>
   </si>
   <si>
-    <t>When using the counterspell reaction, can chose to cast a barrier spell in defence instead of countering. Barriers cast this way have +2 to cast checks.</t>
-  </si>
-  <si>
     <t>Exorcism spells have +5ft radius</t>
   </si>
   <si>
@@ -545,6 +542,51 @@
   </si>
   <si>
     <t>+4 to sources of spirit recovery</t>
+  </si>
+  <si>
+    <t>When using the counterspell reaction, can chose to cast a barrier spell in defence instead of countering. Barriers cast this way have +1 to cast checks.</t>
+  </si>
+  <si>
+    <t>Spells that you successfully bolster gain +1 magnitude</t>
+  </si>
+  <si>
+    <t>When bolstering a hand seal spell, +1 to checks. Gain +2 for talisman checks.</t>
+  </si>
+  <si>
+    <t>Gain the ability to bolster channeling</t>
+  </si>
+  <si>
+    <t>When reacting to an ally, both of you gain +1 spirit armor for the round.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you crit while bolstering, gain an extra turn at the end of initiative. </t>
+  </si>
+  <si>
+    <t>+2 to talisman checks</t>
+  </si>
+  <si>
+    <t>Add extra damage to talisman spells equal to the magnitude of the spell</t>
+  </si>
+  <si>
+    <t>Boosted talisman spells have an extra 10% chance to crit</t>
+  </si>
+  <si>
+    <t>Boosted spells gain an additional +1 magnitude.</t>
+  </si>
+  <si>
+    <t>Gain the spell Resounding Echo. Resounding Echo is automatically cast time in a combat the first time that you cast a spell of magnitude 10 or greater.</t>
+  </si>
+  <si>
+    <t>Resounding Echo</t>
+  </si>
+  <si>
+    <t>10 Any</t>
+  </si>
+  <si>
+    <t>The target is struck with the same amount of damage as your last hit. The talismans used and damage type are the same as the previous spell. This attack cannot be blocked.</t>
+  </si>
+  <si>
+    <t>Deal +4 additional damage with all Bind spells</t>
   </si>
 </sst>
 </file>
@@ -588,11 +630,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323A4BD3-C367-4F55-AFD6-27C708741604}">
   <dimension ref="A1:J126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,14 +969,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
       <c r="G1" t="s">
         <v>71</v>
       </c>
@@ -957,6 +999,9 @@
       <c r="D3" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -965,7 +1010,7 @@
       <c r="D4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -974,28 +1019,28 @@
         <v>91</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="J5" s="4"/>
+        <v>155</v>
+      </c>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>93</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="J6" s="4"/>
+        <v>151</v>
+      </c>
+      <c r="J6" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" t="s">
         <v>72</v>
       </c>
@@ -1008,30 +1053,53 @@
         <v>13</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="J10" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>59</v>
@@ -1042,7 +1110,7 @@
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>63</v>
@@ -1053,7 +1121,7 @@
     </row>
     <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>64</v>
@@ -1076,14 +1144,14 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="G24" t="s">
         <v>74</v>
       </c>
@@ -1093,56 +1161,56 @@
         <v>67</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
       <c r="G32" t="s">
         <v>75</v>
       </c>
@@ -1188,14 +1256,14 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
       <c r="G40" t="s">
         <v>76</v>
       </c>
@@ -1247,14 +1315,14 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
       <c r="G47" t="s">
         <v>77</v>
       </c>
@@ -1272,7 +1340,7 @@
     </row>
     <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>68</v>
@@ -1297,14 +1365,14 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
       <c r="G55" t="s">
         <v>76</v>
       </c>
@@ -1314,7 +1382,7 @@
         <v>112</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>22</v>
@@ -1322,21 +1390,44 @@
     </row>
     <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>115</v>
+        <v>167</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D60" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D61" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
       <c r="G63" t="s">
         <v>76</v>
       </c>
@@ -1349,67 +1440,67 @@
         <v>23</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
       <c r="G72" t="s">
         <v>76</v>
       </c>
@@ -1427,20 +1518,20 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D74" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="D75" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="D76" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1449,16 +1540,16 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
       <c r="G79" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -1471,7 +1562,7 @@
     </row>
     <row r="81" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>98</v>
@@ -1493,14 +1584,14 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
@@ -1510,33 +1601,33 @@
         <v>36</v>
       </c>
       <c r="G88" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
@@ -1546,18 +1637,18 @@
         <v>28</v>
       </c>
       <c r="G96" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
@@ -1567,43 +1658,35 @@
         <v>26</v>
       </c>
       <c r="G104" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="3"/>
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="3"/>
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="3"/>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
-      <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A40:F40"/>
     <mergeCell ref="A103:F103"/>
     <mergeCell ref="A110:F110"/>
     <mergeCell ref="A118:F118"/>
@@ -1614,6 +1697,14 @@
     <mergeCell ref="A79:F79"/>
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A95:F95"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A40:F40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1621,10 +1712,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD8E546-FEBF-4703-B5FC-85F4A1C8F315}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,53 +1810,70 @@
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D8" t="s">
         <v>86</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>